<commit_message>
alteração nome da coluna do relatorio
</commit_message>
<xml_diff>
--- a/DispenserTCC/Relatorio_Dispenser/Relatorio_Dispenser.xlsx
+++ b/DispenserTCC/Relatorio_Dispenser/Relatorio_Dispenser.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vssav\source\repos\DispenserTCC\DispenserTCC\Relatorio_Dispenser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160F021A-F402-4A11-9BE2-344D378F8BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9944C3A2-01F5-4AE1-90D0-990515515D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dispensado" sheetId="1" r:id="rId1"/>
@@ -44,10 +44,10 @@
     <t>Hora</t>
   </si>
   <si>
-    <t>Quantidade Ingerida</t>
-  </si>
-  <si>
     <t>Quantidade Total</t>
+  </si>
+  <si>
+    <t>Quantidade Dispensada</t>
   </si>
 </sst>
 </file>
@@ -474,13 +474,13 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="17.5546875" style="2" customWidth="1"/>
     <col min="4" max="16384" width="8.88671875" style="2"/>
   </cols>
@@ -490,10 +490,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>